<commit_message>
zip2 zip3 + tabusearch
</commit_message>
<xml_diff>
--- a/sprawka/lab2/wyniki.xlsx
+++ b/sprawka/lab2/wyniki.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuperCiuper\Documents\GitHub\PEAproject\sprawka\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7345F4A-38D8-45F5-A25B-52D589FF888F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BE0DC5-10E7-4490-93CB-38A941D41D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{35CB0FE1-15B9-4927-961C-D0566F903D09}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>n</t>
   </si>
@@ -42,25 +42,29 @@
     <t>time</t>
   </si>
   <si>
-    <t>time [ms]</t>
-  </si>
-  <si>
-    <t>expected time [ms]</t>
-  </si>
-  <si>
     <t>KARP</t>
   </si>
   <si>
-    <t>BruteForce [ms]</t>
+    <t>time [s]</t>
   </si>
   <si>
-    <t>Held-Karp</t>
+    <t>expected time [s]</t>
+  </si>
+  <si>
+    <t>BruteForce [s]</t>
+  </si>
+  <si>
+    <t>Held-Karp [s]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,8 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,7 +204,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BruteForce [ms]</c:v>
+                  <c:v>BruteForce [s]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -294,30 +300,30 @@
             <c:numRef>
               <c:f>Sheet1!$F$4:$F$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.40467000000000003</c:v>
+                  <c:v>4.0467000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7264000000000004</c:v>
+                  <c:v>3.7264000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.132999999999996</c:v>
+                  <c:v>4.1132999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>473.62</c:v>
+                  <c:v>0.47361999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5922.9800000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>81866.7</c:v>
+                  <c:v>5.9229800000000008</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000">
+                  <c:v>81.866699999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9C7C-4D1D-925B-1130EA06A915}"/>
@@ -333,7 +339,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Held-Karp</c:v>
+                  <c:v>Held-Karp [s]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -433,25 +439,25 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
-                <c:pt idx="8">
-                  <c:v>61.766800000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1435.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3083.1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>14576.8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>52440.3</c:v>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>6.1766800000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.0000">
+                  <c:v>1.4357</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0000">
+                  <c:v>3.0831</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.000">
+                  <c:v>14.576799999999999</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.000">
+                  <c:v>52.440300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9C7C-4D1D-925B-1130EA06A915}"/>
@@ -568,7 +574,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> [ms]</a:t>
+                  <a:t> [s]</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -603,7 +609,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -743,7 +749,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>time [ms]</c:v>
+                  <c:v>time [s]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -774,10 +780,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$18</c:f>
+              <c:f>Sheet1!$O$7:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -813,38 +819,44 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$7:$P$18</c:f>
+              <c:f>Sheet1!$P$7:$P$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.2495799999999999</c:v>
+                  <c:v>1.2495799999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.766800000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1435.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3083.1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14576.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>52440.3</c:v>
+                  <c:v>6.1766800000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.4357</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>3.0831</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000">
+                  <c:v>14.576799999999999</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000">
+                  <c:v>52.440300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-32F2-4EAA-8D27-2EC80D211D58}"/>
@@ -852,15 +864,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$3</c:f>
+              <c:f>Sheet1!$R$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>expected time [ms]</c:v>
+                  <c:v>expected time [s]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -869,9 +881,11 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2">
-                  <a:alpha val="40000"/>
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -881,12 +895,16 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
-                    <a:alpha val="40000"/>
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -895,10 +913,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$18</c:f>
+              <c:f>Sheet1!$O$7:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -934,63 +952,70 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$7:$Q$18</c:f>
+              <c:f>Sheet1!$R$7:$R$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>9.8303999999999991</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22.369621333333335</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>50.506410666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>113.246208</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>252.35729066666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>559.24053333333336</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1233.125376</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2706.7241813333335</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5916.7648426666665</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12884.901888</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>27962.026666666668</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60487.456085333331</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="2" formatCode="0.0000">
+                  <c:v>9.8303999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0000">
+                  <c:v>2.2369621333333336E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000">
+                  <c:v>5.0506410666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>0.113246208</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>0.25235729066666668</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>0.55924053333333335</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>1.2331253760000001</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000">
+                  <c:v>2.7067241813333336</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0000">
+                  <c:v>5.9167648426666668</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000">
+                  <c:v>12.884901888</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.000">
+                  <c:v>27.96202666666667</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.000">
+                  <c:v>60.487456085333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-32F2-4EAA-8D27-2EC80D211D58}"/>
+              <c16:uniqueId val="{00000001-3CAA-4C7C-9D2E-F49D52EE2043}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1002,6 +1027,175 @@
         <c:smooth val="0"/>
         <c:axId val="1471491792"/>
         <c:axId val="1482048864"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$Q$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>expected time [s]</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:alpha val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2">
+                          <a:alpha val="40000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$O$7:$O$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>28</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$Q$7:$Q$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>9.8303999999999996E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.2369621333333336E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.0506410666666668E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.113246208</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.25235729066666668</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.55924053333333335</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.2331253760000001</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2.7067241813333336</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>5.9167648426666668</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>12.884901888</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>27.96202666666667</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>60.487456085333335</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-32F2-4EAA-8D27-2EC80D211D58}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1471491792"/>
@@ -1011,7 +1205,7 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1100,7 +1294,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> [ms]</a:t>
+                  <a:t> [s]</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -1135,8 +1329,8 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1170,45 +1364,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1217,6 +1372,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
     <c:showDLblsOverMax val="0"/>
@@ -2716,10 +2902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E030250-1702-4C2B-BFB2-8B2C0A8742D5}">
-  <dimension ref="D3:Q21"/>
+  <dimension ref="D3:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,9 +2916,10 @@
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="21.140625" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -2746,7 +2933,7 @@
         <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N3" t="s">
         <v>1</v>
@@ -2755,58 +2942,61 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>4.0467000000000004</v>
       </c>
       <c r="E4">
         <v>9</v>
       </c>
-      <c r="F4">
-        <f>D4/10</f>
-        <v>0.40467000000000003</v>
+      <c r="F4" s="1">
+        <f>D4/10/1000</f>
+        <v>4.0467000000000004E-4</v>
       </c>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>37.264000000000003</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F9" si="0">D5/10</f>
-        <v>3.7264000000000004</v>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F9" si="0">D5/10/1000</f>
+        <v>3.7264000000000004E-3</v>
       </c>
     </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>411.33</v>
       </c>
       <c r="E6">
         <v>11</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>41.132999999999996</v>
+        <v>4.1132999999999996E-2</v>
       </c>
     </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>4736.2</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>473.62</v>
+        <v>0.47361999999999999</v>
       </c>
       <c r="N7">
         <v>12.495799999999999</v>
@@ -2814,44 +3004,45 @@
       <c r="O7">
         <v>15</v>
       </c>
-      <c r="P7">
-        <f>N7/10</f>
-        <v>1.2495799999999999</v>
+      <c r="P7" s="1">
+        <f>N7/10/1000</f>
+        <v>1.2495799999999999E-3</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q6:Q18" si="1">2^O7*O7^2/750000</f>
-        <v>9.8303999999999991</v>
+        <f>2^O7*O7^2/750000/1000</f>
+        <v>9.8303999999999996E-3</v>
       </c>
     </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>59229.8</v>
       </c>
       <c r="E8">
         <v>13</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>5922.9800000000005</v>
+        <v>5.9229800000000008</v>
       </c>
       <c r="O8">
         <v>16</v>
       </c>
+      <c r="P8" s="1"/>
       <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>22.369621333333335</v>
+        <f t="shared" ref="Q8:Q18" si="1">2^O8*O8^2/750000/1000</f>
+        <v>2.2369621333333336E-2</v>
       </c>
     </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>818667</v>
       </c>
       <c r="E9">
         <v>14</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>81866.7</v>
+        <v>81.866699999999994</v>
       </c>
       <c r="N9">
         <v>617.66800000000001</v>
@@ -2859,16 +3050,20 @@
       <c r="O9">
         <v>17</v>
       </c>
-      <c r="P9">
-        <f t="shared" ref="P4:P14" si="2">N9/10</f>
-        <v>61.766800000000003</v>
+      <c r="P9" s="1">
+        <f t="shared" ref="P8:P20" si="2">N9/10/1000</f>
+        <v>6.1766800000000004E-2</v>
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
-        <v>50.506410666666667</v>
+        <v>5.0506410666666668E-2</v>
+      </c>
+      <c r="R9" s="1">
+        <f>Q7</f>
+        <v>9.8303999999999996E-3</v>
       </c>
     </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>3597490</v>
       </c>
@@ -2881,185 +3076,240 @@
       </c>
       <c r="Q10">
         <f t="shared" si="1"/>
-        <v>113.246208</v>
+        <v>0.113246208</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" ref="R10:R20" si="3">Q8</f>
+        <v>2.2369621333333336E-2</v>
       </c>
     </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E11">
         <f>E10+1</f>
         <v>16</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O18" si="3">O10+1</f>
+        <f t="shared" ref="O11:O20" si="4">O10+1</f>
         <v>19</v>
       </c>
       <c r="Q11">
         <f t="shared" si="1"/>
-        <v>252.35729066666667</v>
+        <v>0.25235729066666668</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0506410666666668E-2</v>
       </c>
     </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E12">
-        <f t="shared" ref="E12:E18" si="4">E11+1</f>
+        <f t="shared" ref="E12:E18" si="5">E11+1</f>
         <v>17</v>
       </c>
-      <c r="G12">
-        <f t="shared" ref="G12:G17" si="5">P9</f>
-        <v>61.766800000000003</v>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:G17" si="6">P9</f>
+        <v>6.1766800000000004E-2</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="Q12">
         <f t="shared" si="1"/>
-        <v>559.24053333333336</v>
+        <v>0.55924053333333335</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.113246208</v>
       </c>
     </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="N13">
         <v>14357</v>
       </c>
       <c r="O13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="P13">
-        <f>N13/10</f>
-        <v>1435.7</v>
+        <f t="shared" si="2"/>
+        <v>1.4357</v>
       </c>
       <c r="Q13">
         <f t="shared" si="1"/>
-        <v>1233.125376</v>
+        <v>1.2331253760000001</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25235729066666668</v>
       </c>
     </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="N14">
         <v>30831</v>
       </c>
       <c r="O14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>3083.1</v>
+        <v>3.0831</v>
       </c>
       <c r="Q14">
         <f t="shared" si="1"/>
-        <v>2706.7241813333335</v>
+        <v>2.7067241813333336</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.55924053333333335</v>
       </c>
     </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E15">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="O15">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="Q15">
         <f t="shared" si="1"/>
-        <v>5916.7648426666665</v>
+        <v>5.9167648426666668</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2331253760000001</v>
       </c>
     </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="5"/>
-        <v>1435.7</v>
+      <c r="G16" s="1">
+        <f t="shared" si="6"/>
+        <v>1.4357</v>
       </c>
       <c r="N16">
         <v>145768</v>
       </c>
       <c r="O16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="P16">
-        <f>N16/10</f>
-        <v>14576.8</v>
+      <c r="P16" s="2">
+        <f t="shared" si="2"/>
+        <v>14.576799999999999</v>
       </c>
       <c r="Q16">
         <f t="shared" si="1"/>
-        <v>12884.901888</v>
+        <v>12.884901888</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7067241813333336</v>
       </c>
     </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E17">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="6"/>
+        <v>3.0831</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="5"/>
-        <v>3083.1</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="3"/>
         <v>25</v>
       </c>
+      <c r="P17" s="2"/>
       <c r="Q17">
         <f t="shared" si="1"/>
-        <v>27962.026666666668</v>
+        <v>27.96202666666667</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="3"/>
+        <v>5.9167648426666668</v>
       </c>
     </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
+      <c r="G18" s="2"/>
       <c r="N18">
         <v>524403</v>
       </c>
       <c r="O18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="P18">
-        <f t="shared" ref="P18" si="6">N18/10</f>
-        <v>52440.3</v>
+      <c r="P18" s="2">
+        <f t="shared" si="2"/>
+        <v>52.440300000000001</v>
       </c>
       <c r="Q18">
         <f t="shared" si="1"/>
-        <v>60487.456085333331</v>
+        <v>60.487456085333335</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="3"/>
+        <v>12.884901888</v>
       </c>
     </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E19">
         <f t="shared" ref="E19:E21" si="7">E18+1</f>
         <v>24</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <f t="shared" ref="G19:G21" si="8">P16</f>
-        <v>14576.8</v>
+        <v>14.576799999999999</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="3"/>
+        <v>27.96202666666667</v>
       </c>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E20">
         <f t="shared" si="7"/>
         <v>25</v>
       </c>
+      <c r="G20" s="2"/>
+      <c r="O20">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="3"/>
+        <v>60.487456085333335</v>
+      </c>
     </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E21">
         <f t="shared" si="7"/>
         <v>26</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <f t="shared" si="8"/>
-        <v>52440.3</v>
+        <v>52.440300000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for my love
</commit_message>
<xml_diff>
--- a/sprawka/lab2/wyniki.xlsx
+++ b/sprawka/lab2/wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuperCiuper\Documents\GitHub\PEAproject\sprawka\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BE0DC5-10E7-4490-93CB-38A941D41D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4FE5EB-26F4-4025-90B6-2E2A0617D954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{35CB0FE1-15B9-4927-961C-D0566F903D09}"/>
   </bookViews>
@@ -62,8 +62,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,8 +96,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,6 +214,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -349,6 +350,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -759,6 +761,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -891,25 +894,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1015,7 +1000,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2904,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E030250-1702-4C2B-BFB2-8B2C0A8742D5}">
   <dimension ref="D3:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,7 +3035,7 @@
         <v>17</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" ref="P8:P20" si="2">N9/10/1000</f>
+        <f t="shared" ref="P9:P18" si="2">N9/10/1000</f>
         <v>6.1766800000000004E-2</v>
       </c>
       <c r="Q9">

</xml_diff>